<commit_message>
HybridFrameWork added from Eclipse
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestCase.xlsx
+++ b/src/test/resources/Data/TestCase.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2835" windowWidth="16680" windowHeight="5070"/>
+    <workbookView xWindow="0" yWindow="2835" windowWidth="15675" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:J18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>TestCase No.</t>
   </si>
@@ -80,16 +80,60 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>LINKTEXT</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>SocialMedia</t>
+  </si>
+  <si>
+    <t>GETPAGESOURCE</t>
+  </si>
+  <si>
+    <t>WebSIte</t>
+  </si>
+  <si>
+    <t>GETTITLE</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>sultana@yahoo.com</t>
+  </si>
+  <si>
+    <t>Aemail</t>
+  </si>
+  <si>
+    <t>SCREENSHOT</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>GETTYPEDTEXT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,17 +176,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,23 +504,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,7 +556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -514,65 +576,198 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>